<commit_message>
drive our pubs, first run, no hard output
</commit_message>
<xml_diff>
--- a/pyOurPubs/studentList.xlsx
+++ b/pyOurPubs/studentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/grad_utils/pyOurPubs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5D3651-6AE6-1F41-9A09-4BC0D5FF2345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0C779E-AD6B-AF46-9855-43E48179C311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="500" windowWidth="25040" windowHeight="17500" xr2:uid="{381B9264-B5BB-C64F-A139-4B79C2D4C682}"/>
+    <workbookView xWindow="1600" yWindow="10420" windowWidth="25040" windowHeight="17500" xr2:uid="{381B9264-B5BB-C64F-A139-4B79C2D4C682}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -267,9 +267,6 @@
     <t xml:space="preserve"> Roy</t>
   </si>
   <si>
-    <t>Last Name</t>
-  </si>
-  <si>
     <t>First name</t>
   </si>
   <si>
@@ -378,10 +375,13 @@
     <t>Bowler</t>
   </si>
   <si>
-    <t>PI Last name</t>
-  </si>
-  <si>
     <t>Luo</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>PI last name</t>
   </si>
 </sst>
 </file>
@@ -867,7 +867,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -879,17 +879,17 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="17" t="s">
         <v>78</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>79</v>
       </c>
       <c r="D1" s="17"/>
       <c r="E1" s="17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -897,10 +897,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G2" s="8"/>
     </row>
@@ -909,10 +909,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G3" s="9"/>
     </row>
@@ -921,10 +921,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G4" s="10"/>
     </row>
@@ -936,7 +936,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G5" s="9"/>
     </row>
@@ -948,7 +948,7 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G6" s="9"/>
     </row>
@@ -960,7 +960,7 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G7" s="9"/>
     </row>
@@ -972,7 +972,7 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G8" s="10"/>
     </row>
@@ -981,13 +981,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G9" s="9"/>
     </row>
@@ -999,7 +999,7 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G10" s="10"/>
     </row>
@@ -1011,7 +1011,7 @@
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G11" s="9"/>
     </row>
@@ -1023,7 +1023,7 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G12" s="11"/>
     </row>
@@ -1035,7 +1035,7 @@
         <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G13" s="11"/>
     </row>
@@ -1047,7 +1047,7 @@
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G14" s="11"/>
     </row>
@@ -1059,7 +1059,7 @@
         <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G15" s="11"/>
     </row>
@@ -1068,13 +1068,13 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G16" s="11"/>
     </row>
@@ -1086,7 +1086,7 @@
         <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G17" s="11"/>
     </row>
@@ -1098,7 +1098,7 @@
         <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G18" s="11"/>
     </row>
@@ -1110,7 +1110,7 @@
         <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G19" s="11"/>
     </row>
@@ -1122,7 +1122,7 @@
         <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G20" s="11"/>
     </row>
@@ -1134,7 +1134,7 @@
         <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G21" s="12"/>
     </row>
@@ -1143,13 +1143,13 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
         <v>81</v>
       </c>
-      <c r="C22" t="s">
-        <v>82</v>
-      </c>
       <c r="E22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G22" s="13"/>
     </row>
@@ -1158,10 +1158,10 @@
         <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G23" s="11"/>
     </row>
@@ -1173,7 +1173,7 @@
         <v>38</v>
       </c>
       <c r="E24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G24" s="13"/>
     </row>
@@ -1197,7 +1197,7 @@
         <v>42</v>
       </c>
       <c r="E26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G26" s="13"/>
     </row>
@@ -1209,7 +1209,7 @@
         <v>44</v>
       </c>
       <c r="E27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G27" s="13"/>
     </row>
@@ -1221,7 +1221,7 @@
         <v>46</v>
       </c>
       <c r="E28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G28" s="13"/>
     </row>
@@ -1233,7 +1233,7 @@
         <v>48</v>
       </c>
       <c r="E29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G29" s="13"/>
     </row>
@@ -1245,7 +1245,7 @@
         <v>50</v>
       </c>
       <c r="E30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G30" s="14"/>
     </row>
@@ -1257,7 +1257,7 @@
         <v>52</v>
       </c>
       <c r="E31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G31" s="13"/>
     </row>
@@ -1269,7 +1269,7 @@
         <v>54</v>
       </c>
       <c r="E32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G32" s="13"/>
     </row>
@@ -1281,7 +1281,7 @@
         <v>56</v>
       </c>
       <c r="E33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G33" s="13"/>
     </row>
@@ -1293,7 +1293,7 @@
         <v>57</v>
       </c>
       <c r="E34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G34" s="13"/>
     </row>
@@ -1305,7 +1305,7 @@
         <v>59</v>
       </c>
       <c r="E35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G35" s="13"/>
     </row>
@@ -1317,7 +1317,7 @@
         <v>61</v>
       </c>
       <c r="E36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G36" s="15"/>
     </row>
@@ -1329,7 +1329,7 @@
         <v>63</v>
       </c>
       <c r="E37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G37" s="15"/>
     </row>
@@ -1341,7 +1341,7 @@
         <v>65</v>
       </c>
       <c r="E38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G38" s="13"/>
     </row>
@@ -1353,7 +1353,7 @@
         <v>67</v>
       </c>
       <c r="E39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G39" s="13"/>
     </row>
@@ -1365,7 +1365,7 @@
         <v>69</v>
       </c>
       <c r="E40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G40" s="15"/>
     </row>
@@ -1377,7 +1377,7 @@
         <v>71</v>
       </c>
       <c r="E41" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G41" s="15"/>
     </row>
@@ -1389,7 +1389,7 @@
         <v>73</v>
       </c>
       <c r="E42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G42" s="15"/>
     </row>
@@ -1401,7 +1401,7 @@
         <v>75</v>
       </c>
       <c r="E43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G43" s="13"/>
     </row>
@@ -1413,7 +1413,7 @@
         <v>76</v>
       </c>
       <c r="E44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G44" s="16"/>
     </row>

</xml_diff>